<commit_message>
added prompt file and update prompting
</commit_message>
<xml_diff>
--- a/output/Roster_Output.xlsx
+++ b/output/Roster_Output.xlsx
@@ -533,12 +533,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Termination Notification</t>
+          <t>Term</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Unknown Provider</t>
+          <t>Rchn &amp; Rcssd</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -578,10 +578,14 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>FFS/PPO/ACO/HMO/Medi-Cal</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr"/>
+          <t>["FFS/PPO/ACO/HMO/Medi-Cal"]</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Information not found</t>
+        </is>
+      </c>
       <c r="L2" t="inlineStr">
         <is>
           <t>Information not found</t>
@@ -619,19 +623,19 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>unknown@example.com</t>
+          <t>prajay.sapkale@hilabs.com</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Term</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cyrus Hendricks, M.D</t>
+          <t>Cyrus Hendricks, M.D.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -641,7 +645,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>458888885</t>
+          <t>4568888895</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -654,7 +658,11 @@
           <t>Internal Medicine</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>207R00000X</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
           <t>09/01/2025</t>
@@ -667,7 +675,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>["PPG's", "Medicare"]</t>
+          <t>PPG#’s, Medicare</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -677,7 +685,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Mercian Medical Group</t>
+          <t>Mercian Medical Group – 0P4</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -712,19 +720,19 @@
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>prajay.sapkale@hilabs.com</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Term</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Paul Mcmallan, Md</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -809,7 +817,7 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>unknown@example.com</t>
+          <t>p rajay.sapkale@hilabs.com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove whatwg-fetch polyfill and related files; update run_parser.py to fix field extraction and normalization; generate output Excel file; delete obsolete test_parser.py.
</commit_message>
<xml_diff>
--- a/output/Roster_Output.xlsx
+++ b/output/Roster_Output.xlsx
@@ -538,12 +538,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Rchn &amp; Rcssd</t>
+          <t>Cole Garrett</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>1222222250</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -558,7 +558,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Pediatric Emergency Medicine</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -568,12 +568,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>08/01/2025</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>08/01/2025</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -581,11 +581,7 @@
           <t>["FFS/PPO/ACO/HMO/Medi-Cal"]</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Information not found</t>
-        </is>
-      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
           <t>Information not found</t>
@@ -645,7 +641,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>4568888895</t>
+          <t>458888885</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -675,17 +671,13 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>PPG#’s, Medicare</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>1014</t>
-        </is>
-      </c>
+          <t>PPG#'s, Medicare, Commercial HMO</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Mercian Medical Group – 0P4</t>
+          <t>Mercian Medical Group - 1014</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -817,7 +809,7 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>p rajay.sapkale@hilabs.com</t>
+          <t>prajay.sapkale@hilabs.com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add whatwg-fetch polyfill and update parser normalization logic
- Introduced whatwg-fetch polyfill with UMD and ES module support.
- Added Flow type definitions for fetch and related classes.
- Updated package.json for whatwg-fetch with necessary dependencies and scripts.
- Modified normalizer.py to enhance name normalization by extracting leading alphabetic substrings.
- Updated run_parser.py to normalize additional fields including Provider NPI, PPG ID, Phone Number, and Fax Number.
- Enhanced system prompt to include detailed schema fields with descriptions and examples for better extraction clarity.
</commit_message>
<xml_diff>
--- a/output/Roster_Output.xlsx
+++ b/output/Roster_Output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,92 +441,82 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Transaction Attribute</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Effective Date</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Termination Date</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Termination Reason</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Provider Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>NPI</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Provider NPI</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Provider Specialty</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>State License</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Organization Name</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>TIN</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>State License</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Specialty</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Subspecialty</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Effective Date</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Termination Date</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Lines of Business</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>PPG</t>
-        </is>
-      </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Organization Name</t>
+          <t>Group NPI</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Address</t>
+          <t>Complete Address</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>City</t>
+          <t>Phone Number</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>State</t>
+          <t>Fax Number</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>ZIP</t>
+          <t>PPG ID</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Phone</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Fax</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Email</t>
+          <t>Lines of Business(Medicare/Commercial/Medical)</t>
         </is>
       </c>
     </row>
@@ -538,50 +528,54 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cole Garrett</t>
+          <t>Provider Name</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Information not found</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>08/01/2025</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Voluntary</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Cole</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>1222222250</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Pediatric Emergency Medicine</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Information not found</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Rchn</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>821111113</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Information not found</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Pediatric Emergency Medicine</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Information not found</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>08/01/2025</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>08/01/2025</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>["FFS/PPO/ACO/HMO/Medi-Cal"]</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
           <t>Information not found</t>
@@ -609,17 +603,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Information not found</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Information not found</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>prajay.sapkale@hilabs.com</t>
+          <t>FFS/PPO/ACO/HMO/Medi-Cal</t>
         </is>
       </c>
     </row>
@@ -631,53 +615,57 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cyrus Hendricks, M.D.</t>
+          <t>Provider</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>09/01/2025</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Information not found</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Information not found</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Cyrus</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>1164444443</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Internal Medicine</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>D66661</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Mercian</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>458888885</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>D66661</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Internal Medicine</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>207R00000X</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>09/01/2025</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Information not found</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>PPG#'s, Medicare, Commercial HMO</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Mercian Medical Group - 1014</t>
+          <t>1999999997</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -697,39 +685,29 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>041104</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Information not found</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>Information not found</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>prajay.sapkale@hilabs.com</t>
+          <t>Medicare, PPG#’s, Commercial HMO</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Term</t>
+          <t>Update</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Paul Mcmallan, Md</t>
+          <t>Provider</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>09/22/2025</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -744,7 +722,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -754,7 +732,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>09/22/2025</t>
+          <t>Information not found</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -764,7 +742,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Hilabs</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -800,16 +778,6 @@
       <c r="Q4" t="inlineStr">
         <is>
           <t>Information not found</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>Information not found</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>prajay.sapkale@hilabs.com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor field extraction logic: rename termination fields to 'Term Date' and 'Term Reason'; update extraction and normalization in run_parser.py; modify system prompt for consistency.
</commit_message>
<xml_diff>
--- a/output/Roster_Output.xlsx
+++ b/output/Roster_Output.xlsx
@@ -451,12 +451,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Termination Date</t>
+          <t>Term Date</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Termination Reason</t>
+          <t>Term Reason</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -528,7 +528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Provider Name</t>
+          <t>Provider</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -548,7 +548,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Cole</t>
+          <t>Cole Garrett</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -568,12 +568,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Rchn</t>
+          <t>RCHN &amp; RCSSD</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>821111113</t>
+          <t>82-1111113</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -620,14 +620,14 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Information not found</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>09/01/2025</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Information not found</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>Information not found</t>
@@ -635,7 +635,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Cyrus</t>
+          <t>Cyrus Hendricks, M.D.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Internal Medicine</t>
+          <t>Internal Medicine 207R00000X</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -655,12 +655,12 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Mercian</t>
+          <t>Mercian Medical Group – P04</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>458888885</t>
+          <t>45-8888885</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -685,24 +685,24 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>041104</t>
+          <t>P04, 1104, 569</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Medicare, PPG#’s, Commercial HMO</t>
+          <t>Medicare, Commercial HMO</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Update</t>
+          <t>Add</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Provider</t>
+          <t>Primary Practice Location</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -722,7 +722,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Paul Mcmallan, MD</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -742,7 +742,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Hilabs</t>
+          <t>HILABS</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -772,12 +772,12 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>P01, P03</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Information not found</t>
+          <t>Medicare, Medical</t>
         </is>
       </c>
     </row>

</xml_diff>